<commit_message>
Calculate the duration of lesson plans according to the steps duration
</commit_message>
<xml_diff>
--- a/public/assets/download/edflix_lesson_plan.xlsx
+++ b/public/assets/download/edflix_lesson_plan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/edflix-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7710F7E4-765B-3F40-8819-08B5C89ECD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201AA345-EE74-BD4C-B0A6-BFE6ADE85AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8720" yWindow="4840" windowWidth="20840" windowHeight="12040" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
+    <workbookView xWindow="5740" yWindow="6260" windowWidth="20840" windowHeight="12040" activeTab="1" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>topic</t>
   </si>
@@ -78,6 +79,33 @@
   </si>
   <si>
     <t>S1</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>teacher_activity</t>
+  </si>
+  <si>
+    <t>student_activity</t>
+  </si>
+  <si>
+    <t>knowledge</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>assessment_criteria</t>
+  </si>
+  <si>
+    <t>facilitator_note</t>
   </si>
 </sst>
 </file>
@@ -431,7 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B869820A-E3BD-FB44-8DB2-FA814F95DFBF}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -530,4 +558,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F8D896-B8D0-644E-9C89-5B9F5B02CA90}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="18.5" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Steps sheet to the upload together with preliminary data
</commit_message>
<xml_diff>
--- a/public/assets/download/edflix_lesson_plan.xlsx
+++ b/public/assets/download/edflix_lesson_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/edflix-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201AA345-EE74-BD4C-B0A6-BFE6ADE85AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7042A7D0-9D3A-754D-9404-EEAE29831D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="6260" windowWidth="20840" windowHeight="12040" activeTab="1" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
+    <workbookView xWindow="5880" yWindow="2700" windowWidth="20840" windowHeight="12040" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>topic</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Number</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
     <t>step</t>
   </si>
   <si>
@@ -106,6 +103,27 @@
   </si>
   <si>
     <t>facilitator_note</t>
+  </si>
+  <si>
+    <t>Give quiz according to previous lesson</t>
+  </si>
+  <si>
+    <t>Answering Questions</t>
+  </si>
+  <si>
+    <t>previous topic</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Understand previous topic</t>
+  </si>
+  <si>
+    <t>Answers</t>
+  </si>
+  <si>
+    <t>Quiz questions</t>
   </si>
 </sst>
 </file>
@@ -459,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B869820A-E3BD-FB44-8DB2-FA814F95DFBF}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -521,9 +539,6 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
       <c r="D2">
         <v>10</v>
       </c>
@@ -562,50 +577,73 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F8D896-B8D0-644E-9C89-5B9F5B02CA90}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
     <col min="9" max="9" width="18.5" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update lesson plan excel template
</commit_message>
<xml_diff>
--- a/public/assets/download/edflix_lesson_plan.xlsx
+++ b/public/assets/download/edflix_lesson_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/edflix-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7042A7D0-9D3A-754D-9404-EEAE29831D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04EC308-A7ED-A24C-894C-720A8D3976D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="2700" windowWidth="20840" windowHeight="12040" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
+    <workbookView xWindow="5880" yWindow="2700" windowWidth="20840" windowHeight="12040" activeTab="1" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>topic</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Quiz questions</t>
+  </si>
+  <si>
+    <t>S1</t>
   </si>
 </sst>
 </file>
@@ -477,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B869820A-E3BD-FB44-8DB2-FA814F95DFBF}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -539,6 +542,9 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
       <c r="D2">
         <v>10</v>
       </c>
@@ -571,6 +577,15 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{94C0EC54-6424-CB47-A742-6829F7BDCFBA}">
+      <formula1>"S1,S2,S3,S4,S5,S6"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not Allowed" error="Please enter a number from 1 and 1000" sqref="D2" xr:uid="{76A3A707-812F-2D49-BFA0-0D871D0AECB0}">
+      <formula1>1</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -579,14 +594,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71F8D896-B8D0-644E-9C89-5B9F5B02CA90}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
     <col min="9" max="9" width="18.5" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
   </cols>
@@ -624,6 +640,12 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Cleanup and Adding the preview of lesson plans
</commit_message>
<xml_diff>
--- a/public/assets/download/edflix_lesson_plan.xlsx
+++ b/public/assets/download/edflix_lesson_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/edflix-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04EC308-A7ED-A24C-894C-720A8D3976D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550687FD-F507-334C-930C-1645E8A8E5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5880" yWindow="2700" windowWidth="20840" windowHeight="12040" activeTab="1" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>topic</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>S1</t>
+  </si>
+  <si>
+    <t>step_values</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,7 +630,7 @@
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Add extended session time
</commit_message>
<xml_diff>
--- a/public/assets/download/edflix_lesson_plan.xlsx
+++ b/public/assets/download/edflix_lesson_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/edflix-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51D5597-4DB6-3348-9950-848300CC72DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D06404-21D1-AA41-886E-08950EE48B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5880" yWindow="2700" windowWidth="20840" windowHeight="12040" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
   </bookViews>

</xml_diff>

<commit_message>
Add competency and school term to lesson plan upload
</commit_message>
<xml_diff>
--- a/public/assets/download/edflix_lesson_plan.xlsx
+++ b/public/assets/download/edflix_lesson_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/edflix-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C23C11D1-B8AE-6D49-978A-62E972AA4CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5075152D-CADC-2E45-9B64-F3B7709CE3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5880" yWindow="2700" windowWidth="20840" windowHeight="12040" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
   </bookViews>
@@ -21,20 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>topic</t>
   </si>
@@ -133,6 +125,9 @@
   </si>
   <si>
     <t>term</t>
+  </si>
+  <si>
+    <t>competency</t>
   </si>
 </sst>
 </file>
@@ -484,23 +479,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B869820A-E3BD-FB44-8DB2-FA814F95DFBF}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" customWidth="1"/>
-    <col min="10" max="11" width="24.6640625" customWidth="1"/>
-    <col min="12" max="13" width="21.83203125" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" customWidth="1"/>
+    <col min="6" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="11" max="12" width="24.6640625" customWidth="1"/>
+    <col min="13" max="14" width="21.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -517,34 +512,37 @@
         <v>32</v>
       </c>
       <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -585,6 +583,9 @@
         <v>13</v>
       </c>
       <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add activity_aim on lesson plans
</commit_message>
<xml_diff>
--- a/public/assets/download/edflix_lesson_plan.xlsx
+++ b/public/assets/download/edflix_lesson_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/edflix-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5075152D-CADC-2E45-9B64-F3B7709CE3C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632181EF-BE78-B441-808A-2728EA5E0832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5880" yWindow="2700" windowWidth="20840" windowHeight="12040" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>topic</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>competency</t>
+  </si>
+  <si>
+    <t>activity_aim</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B869820A-E3BD-FB44-8DB2-FA814F95DFBF}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,7 +498,7 @@
     <col min="15" max="15" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -541,8 +544,11 @@
       <c r="O1" t="s">
         <v>12</v>
       </c>
+      <c r="P1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -586,6 +592,9 @@
         <v>13</v>
       </c>
       <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add activity aim to LP example
</commit_message>
<xml_diff>
--- a/public/assets/download/edflix_lesson_plan.xlsx
+++ b/public/assets/download/edflix_lesson_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/edflix-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632181EF-BE78-B441-808A-2728EA5E0832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6C8742-CBCC-A84B-BCC5-498CE2D05BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5880" yWindow="2700" windowWidth="20840" windowHeight="12040" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update the upload LP with female and male learner fields
</commit_message>
<xml_diff>
--- a/public/assets/download/edflix_lesson_plan.xlsx
+++ b/public/assets/download/edflix_lesson_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/edflix-laravel/public/assets/download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6C8742-CBCC-A84B-BCC5-498CE2D05BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF46C1E8-C38E-D145-A129-D781FFA9F945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5880" yWindow="2700" windowWidth="20840" windowHeight="12040" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>topic</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>activity_aim</t>
+  </si>
+  <si>
+    <t>female_learners</t>
+  </si>
+  <si>
+    <t>male_learners</t>
   </si>
 </sst>
 </file>
@@ -482,23 +488,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B869820A-E3BD-FB44-8DB2-FA814F95DFBF}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="21.33203125" customWidth="1"/>
-    <col min="11" max="12" width="24.6640625" customWidth="1"/>
-    <col min="13" max="14" width="21.83203125" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="8" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" customWidth="1"/>
+    <col min="13" max="14" width="24.6640625" customWidth="1"/>
+    <col min="15" max="16" width="21.83203125" customWidth="1"/>
+    <col min="17" max="17" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -512,43 +521,49 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -562,14 +577,14 @@
         <v>10</v>
       </c>
       <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
@@ -595,6 +610,12 @@
         <v>13</v>
       </c>
       <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -603,7 +624,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{94C0EC54-6424-CB47-A742-6829F7BDCFBA}">
       <formula1>"S1,S2,S3,S4,S5,S6"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not Allowed" error="Please enter a number from 1 and 1000" sqref="D2:E2" xr:uid="{76A3A707-812F-2D49-BFA0-0D871D0AECB0}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not Allowed" error="Please enter a number from 1 and 1000" sqref="D2:G2" xr:uid="{76A3A707-812F-2D49-BFA0-0D871D0AECB0}">
       <formula1>1</formula1>
       <formula2>1000</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Handle the Female and Male learner comments and editing
</commit_message>
<xml_diff>
--- a/public/assets/download/edflix_lesson_plan.xlsx
+++ b/public/assets/download/edflix_lesson_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/LGIHE/Dev/edflix-laravel/public/assets/download/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caleb/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF46C1E8-C38E-D145-A129-D781FFA9F945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9902F1-2A87-C34E-B3CE-548D5B8BE6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5880" yWindow="2700" windowWidth="20840" windowHeight="12040" xr2:uid="{53A2B662-9E11-704B-ACAC-705962D637ED}"/>
   </bookViews>
@@ -16,10 +16,20 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -491,14 +501,13 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="6" width="17" customWidth="1"/>
     <col min="8" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="15.6640625" customWidth="1"/>
     <col min="12" max="12" width="21.33203125" customWidth="1"/>
@@ -518,13 +527,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
       </c>
       <c r="G1" t="s">
         <v>32</v>
@@ -574,13 +583,14 @@
         <v>30</v>
       </c>
       <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <f>SUM(D2+E2)</f>
         <v>10</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
       </c>
       <c r="G2">
         <v>1</v>

</xml_diff>